<commit_message>
added populations to file; deleted Columbus b/c not in location information file
</commit_message>
<xml_diff>
--- a/Monthly-Electricity-Consumption-for-Major-US-Cities.xlsx
+++ b/Monthly-Electricity-Consumption-for-Major-US-Cities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megan\Downloads\final-project-MegaBrett\final-project-MegaBrett\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megan\Downloads\final-project-MegaBrett\final-project-final-megabrett\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39CDD1C-1170-474E-B54A-08C88C47BABD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4299E7B-2944-4DD1-B6CF-1D97F5EFEAAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2064" yWindow="912" windowWidth="16056" windowHeight="11052" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3492" yWindow="684" windowWidth="16056" windowHeight="11052" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Statistic as Excel data file</t>
   </si>
@@ -101,12 +101,6 @@
     <t>807951</t>
   </si>
   <si>
-    <t>Monthly electricity consumption in major U.S. cities 2017</t>
-  </si>
-  <si>
-    <t>Average monthly usage in kilowatt hours</t>
-  </si>
-  <si>
     <t>Miami</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
   </si>
   <si>
     <t>Washington, D.C.</t>
-  </si>
-  <si>
-    <t>Columbus</t>
   </si>
   <si>
     <t>Denver</t>
@@ -218,7 +209,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -235,12 +226,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
@@ -738,149 +723,169 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="100.6640625" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" customWidth="1"/>
+    <col min="1" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="B1" s="7">
+        <v>1125</v>
+      </c>
+      <c r="C1">
+        <v>0.45400000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="7">
+        <v>905</v>
+      </c>
+      <c r="C2">
+        <v>1.63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="9">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="7">
+        <v>879</v>
+      </c>
+      <c r="C3">
+        <v>0.84199999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="9">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="7">
+        <v>837</v>
+      </c>
+      <c r="C4">
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="9">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
+        <v>788</v>
+      </c>
+      <c r="C5">
+        <v>0.64800000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="9">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
+        <v>735</v>
+      </c>
+      <c r="C6">
+        <v>4.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="9">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
+        <v>669</v>
+      </c>
+      <c r="C7">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="9">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
+        <v>613</v>
+      </c>
+      <c r="C8">
+        <v>0.70199999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="9">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
+        <v>475</v>
+      </c>
+      <c r="C9">
+        <v>0.70499999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="9">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
+        <v>394</v>
+      </c>
+      <c r="C10">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="9">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>380</v>
+      </c>
+      <c r="C11">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="9">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="7">
+        <v>326</v>
+      </c>
+      <c r="C12">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="9">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
+        <v>304</v>
+      </c>
+      <c r="C13">
+        <v>8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="9">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="9">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="9">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="9">
+      <c r="B14" s="7">
         <v>261</v>
+      </c>
+      <c r="C14">
+        <v>0.88400000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>